<commit_message>
en procesod de añadir un contacto
</commit_message>
<xml_diff>
--- a/file.xlsx
+++ b/file.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t xml:space="preserve">NOMBRE EMPRESA</t>
   </si>
@@ -98,6 +98,36 @@
   </si>
   <si>
     <t xml:space="preserve">periodico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mercadolibre4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ml.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compras online</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MC6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MC7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jhjhjhhj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ghfghfg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thrtyrtyrt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUKIS 4444</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MARCO ANTONIO 444</t>
   </si>
 </sst>
 </file>
@@ -328,16 +358,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.02"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.29"/>
@@ -450,13 +480,50 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
agregando contactos no existentes en el CRM
</commit_message>
<xml_diff>
--- a/file.xlsx
+++ b/file.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
   <si>
     <t xml:space="preserve">NOMBRE EMPRESA</t>
   </si>
@@ -100,7 +100,13 @@
     <t xml:space="preserve">periodico</t>
   </si>
   <si>
-    <t xml:space="preserve">mercadolibre4</t>
+    <t xml:space="preserve">manuel@eltiempo.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">precualification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mercado libre</t>
   </si>
   <si>
     <t xml:space="preserve">ml.com</t>
@@ -109,25 +115,37 @@
     <t xml:space="preserve">compras online</t>
   </si>
   <si>
-    <t xml:space="preserve">MC6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MC7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jhjhjhhj</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ghfghfg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">thrtyrtyrt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BUKIS 4444</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MARCO ANTONIO 444</t>
+    <t xml:space="preserve">enrique lozano</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kike@mc.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">falabella</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fb.comq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ventas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enrique osorio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">latti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lt.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">leche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fabiola martinez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fabiola@eltiempo.com</t>
   </si>
 </sst>
 </file>
@@ -206,12 +224,24 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF729FCF"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -248,7 +278,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -265,11 +295,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -278,6 +316,22 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -308,7 +362,7 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF729FCF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
@@ -361,7 +415,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -404,73 +458,73 @@
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="4" t="n">
+      <c r="E2" s="5" t="n">
         <v>999999999</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="7" t="n">
+      <c r="E3" s="9" t="n">
         <v>42354354</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="7" t="n">
+      <c r="E4" s="9" t="n">
         <v>3432432</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="12" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="0" t="s">
@@ -479,51 +533,86 @@
       <c r="C5" s="0" t="s">
         <v>25</v>
       </c>
+      <c r="D5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>543534543</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>26</v>
+      <c r="A6" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>534545345</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="0" t="s">
         <v>27</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>3454354</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>30</v>
+        <v>37</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>4324324</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>35</v>
-      </c>
-    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1516,6 +1605,10 @@
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" display="hp.com"/>
     <hyperlink ref="B4" r:id="rId2" display="surtifruver.com"/>
+    <hyperlink ref="F5" r:id="rId3" display="manuel@eltiempo"/>
+    <hyperlink ref="F6" r:id="rId4" display="kike@mc.com"/>
+    <hyperlink ref="F7" r:id="rId5" display="manuel@eltiempo.com"/>
+    <hyperlink ref="F8" r:id="rId6" display="fabiola@eltiempo.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>

</xml_diff>

<commit_message>
problema con hubspot cache
</commit_message>
<xml_diff>
--- a/file.xlsx
+++ b/file.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
   <si>
     <t xml:space="preserve">NOMBRE EMPRESA</t>
   </si>
@@ -31,10 +31,13 @@
     <t xml:space="preserve">INDUSTRIA</t>
   </si>
   <si>
-    <t xml:space="preserve">NOMBRE DEL CONTACTO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TELEFONO CONTACTO </t>
+    <t xml:space="preserve">PRIMER NOMBRE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEGUNDO NOMBRE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TELEFONO DE CONTACTO</t>
   </si>
   <si>
     <t xml:space="preserve">EMAIL CONTACTO</t>
@@ -43,109 +46,136 @@
     <t xml:space="preserve">ETAPA</t>
   </si>
   <si>
-    <t xml:space="preserve">Alpina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">alpina.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lacteos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cristian carreño</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cristiancarreño@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pre qualification</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hp.com</t>
+    <t xml:space="preserve">colanta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">colanta.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">leche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mauro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fabian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mauro@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">precualification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cocosete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cocosete.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alimento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pedrooo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iguera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">naaawewe@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">electricaribe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">electricaribe.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">electricidad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aguilera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">costeño</t>
+  </si>
+  <si>
+    <t xml:space="preserve">crcaguilerapo@pornhub.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfsdfdsf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fvsdfsdfsd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsdfsdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dsfsdfds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsdfds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ggdfgfdgfd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fgdfgdgdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">club social </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cs.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">porno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">polanco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">crc@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vbgfhfghf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">huawei</t>
+  </si>
+  <si>
+    <t xml:space="preserve">huawei.comm</t>
   </si>
   <si>
     <t xml:space="preserve">tecnologia</t>
   </si>
   <si>
-    <t xml:space="preserve">manuel plazas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">manuel@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">surtifruver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">surtifruver.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">frutas y verduras</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pedro rivera</t>
-  </si>
-  <si>
-    <t xml:space="preserve">peter@surtifruver.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eltiempo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eltiempo.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">periodico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">manuel@eltiempo.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">precualification</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mercado libre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ml.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">compras online</t>
-  </si>
-  <si>
-    <t xml:space="preserve">enrique lozano</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kike@mc.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">falabella</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fb.comq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ventas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">enrique osorio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">latti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lt.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">leche</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fabiola martinez</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fabiola@eltiempo.com</t>
+    <t xml:space="preserve">Mike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sgurt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mark@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsdfddfsdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exitooo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">éxito.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eleekk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dsss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exitooo@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -216,32 +246,18 @@
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Cambria"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF729FCF"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -278,7 +294,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -295,7 +311,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -303,11 +319,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -319,19 +331,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -362,7 +366,7 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF729FCF"/>
+      <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
@@ -412,23 +416,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1000"/>
+  <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.67"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="24.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="8" style="0" width="8.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="24.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="9" style="0" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="28" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -450,163 +455,193 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="5" t="n">
-        <v>999999999</v>
-      </c>
-      <c r="F2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>12</v>
+      </c>
+      <c r="F2" s="4" t="n">
+        <v>4423432</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="8" t="n">
+        <v>4342343333</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>14</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="9" t="n">
-        <v>42354354</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="9" t="n">
-        <v>3432432</v>
-      </c>
-      <c r="F4" s="10" t="s">
+      <c r="B4" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="9" t="s">
-        <v>12</v>
+      <c r="C4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="8" t="n">
+        <v>5767567</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12" t="s">
-        <v>23</v>
+      <c r="A5" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>543534543</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="10" t="n">
+        <v>43543543</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="s">
-        <v>28</v>
+      <c r="A6" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>534545345</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>27</v>
+        <v>35</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="10" t="n">
+        <v>545345345</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>33</v>
+      <c r="A7" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <v>3454354</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>26</v>
+        <v>41</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="10" t="n">
+        <v>53544564</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>37</v>
+      <c r="A8" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="0" t="n">
-        <v>4324324</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>41</v>
+        <v>48</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="10" t="n">
+        <v>5454545322</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1603,12 +1638,12 @@
     <row r="1000" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="hp.com"/>
-    <hyperlink ref="B4" r:id="rId2" display="surtifruver.com"/>
-    <hyperlink ref="F5" r:id="rId3" display="manuel@eltiempo"/>
-    <hyperlink ref="F6" r:id="rId4" display="kike@mc.com"/>
-    <hyperlink ref="F7" r:id="rId5" display="manuel@eltiempo.com"/>
-    <hyperlink ref="F8" r:id="rId6" display="fabiola@eltiempo.com"/>
+    <hyperlink ref="G2" r:id="rId1" display="mauro@gmail.com"/>
+    <hyperlink ref="G3" r:id="rId2" display="naaawewe@gmail.com"/>
+    <hyperlink ref="G4" r:id="rId3" display="crcaguilerapo@pornhub.com"/>
+    <hyperlink ref="G6" r:id="rId4" display="crc@gmail.com"/>
+    <hyperlink ref="G7" r:id="rId5" display="mark@gmail.com"/>
+    <hyperlink ref="G8" r:id="rId6" display="exitooo@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>

</xml_diff>

<commit_message>
creando compania y contacto desenlazados
</commit_message>
<xml_diff>
--- a/file.xlsx
+++ b/file.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="67">
   <si>
     <t xml:space="preserve">NOMBRE EMPRESA</t>
   </si>
@@ -176,6 +176,51 @@
   </si>
   <si>
     <t xml:space="preserve">exitooo@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rappi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rappi.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">delivery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mateus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uribe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mateus@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rappi2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mateus2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">correo1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rappi3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">correo3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rappi4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">correo4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rappi5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">correo5@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -185,7 +230,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -245,12 +290,6 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -294,7 +333,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -315,19 +354,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -419,7 +446,7 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
+      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -484,82 +511,82 @@
       <c r="G2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="8" t="n">
+      <c r="F3" s="6" t="n">
         <v>4342343333</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="8" t="n">
+      <c r="F4" s="6" t="n">
         <v>5767567</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="10" t="n">
+      <c r="F5" s="7" t="n">
         <v>43543543</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="7" t="s">
         <v>32</v>
       </c>
       <c r="H5" s="0" t="s">
@@ -567,25 +594,25 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="10" t="n">
+      <c r="F6" s="7" t="n">
         <v>545345345</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="7" t="s">
         <v>38</v>
       </c>
       <c r="H6" s="0" t="s">
@@ -593,25 +620,25 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="7" t="s">
         <v>40</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="10" t="n">
+      <c r="F7" s="7" t="n">
         <v>53544564</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="7" t="s">
         <v>45</v>
       </c>
       <c r="H7" s="0" t="s">
@@ -619,36 +646,161 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="7" t="s">
         <v>47</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="F8" s="10" t="n">
+      <c r="F8" s="7" t="n">
         <v>5454545322</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="7" t="s">
         <v>51</v>
       </c>
       <c r="H8" s="0" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>543545</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>543545</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>543545</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>543545</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>543545</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1644,6 +1796,8 @@
     <hyperlink ref="G6" r:id="rId4" display="crc@gmail.com"/>
     <hyperlink ref="G7" r:id="rId5" display="mark@gmail.com"/>
     <hyperlink ref="G8" r:id="rId6" display="exitooo@gmail.com"/>
+    <hyperlink ref="G9" r:id="rId7" display="mateus@gmail.com"/>
+    <hyperlink ref="G13" r:id="rId8" display="correo5@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>

</xml_diff>

<commit_message>
haciendo union entre empresa y contacto
</commit_message>
<xml_diff>
--- a/file.xlsx
+++ b/file.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="71">
   <si>
     <t xml:space="preserve">NOMBRE EMPRESA</t>
   </si>
@@ -118,7 +118,7 @@
     <t xml:space="preserve">fsdfds</t>
   </si>
   <si>
-    <t xml:space="preserve">ggdfgfdgfd</t>
+    <t xml:space="preserve">juanluis@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">fgdfgdgdf</t>
@@ -202,25 +202,37 @@
     <t xml:space="preserve">mateus2</t>
   </si>
   <si>
-    <t xml:space="preserve">correo1</t>
+    <t xml:space="preserve">correo1@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">rappi3</t>
   </si>
   <si>
-    <t xml:space="preserve">correo3</t>
+    <t xml:space="preserve">correo3@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">rappi4</t>
   </si>
   <si>
-    <t xml:space="preserve">correo4</t>
+    <t xml:space="preserve">gggg@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">rappi5</t>
   </si>
   <si>
     <t xml:space="preserve">correo5@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rappi6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">correo6@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rappi7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">correo7@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -446,7 +458,7 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -801,8 +813,58 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>543545</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>543545</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1793,11 +1855,17 @@
     <hyperlink ref="G2" r:id="rId1" display="mauro@gmail.com"/>
     <hyperlink ref="G3" r:id="rId2" display="naaawewe@gmail.com"/>
     <hyperlink ref="G4" r:id="rId3" display="crcaguilerapo@pornhub.com"/>
-    <hyperlink ref="G6" r:id="rId4" display="crc@gmail.com"/>
-    <hyperlink ref="G7" r:id="rId5" display="mark@gmail.com"/>
-    <hyperlink ref="G8" r:id="rId6" display="exitooo@gmail.com"/>
-    <hyperlink ref="G9" r:id="rId7" display="mateus@gmail.com"/>
-    <hyperlink ref="G13" r:id="rId8" display="correo5@gmail.com"/>
+    <hyperlink ref="G5" r:id="rId4" display="juanluis@gmail.com"/>
+    <hyperlink ref="G6" r:id="rId5" display="crc@gmail.com"/>
+    <hyperlink ref="G7" r:id="rId6" display="mark@gmail.com"/>
+    <hyperlink ref="G8" r:id="rId7" display="exitooo@gmail.com"/>
+    <hyperlink ref="G9" r:id="rId8" display="mateus@gmail.com"/>
+    <hyperlink ref="G10" r:id="rId9" display="correo1@gmail.com"/>
+    <hyperlink ref="G11" r:id="rId10" display="correo3@gmail.com"/>
+    <hyperlink ref="G12" r:id="rId11" display="gggg@gmail.com"/>
+    <hyperlink ref="G13" r:id="rId12" display="correo5@gmail.com"/>
+    <hyperlink ref="G14" r:id="rId13" display="correo6@gmail.com"/>
+    <hyperlink ref="G15" r:id="rId14" display="correo7@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>

</xml_diff>

<commit_message>
funcionando hasta union de empresa y contacto
</commit_message>
<xml_diff>
--- a/file.xlsx
+++ b/file.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t xml:space="preserve">NOMBRE EMPRESA</t>
   </si>
@@ -46,193 +46,61 @@
     <t xml:space="preserve">ETAPA</t>
   </si>
   <si>
-    <t xml:space="preserve">colanta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">colanta.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">leche</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mauro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fabian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mauro@gmail.com</t>
+    <t xml:space="preserve">puntosamarillo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">puntosamarillo.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pinturas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hernandez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mario@puntosamarillo.com</t>
   </si>
   <si>
     <t xml:space="preserve">precualification</t>
   </si>
   <si>
-    <t xml:space="preserve">cocosete</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cocosete.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">alimento</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pedrooo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">iguera</t>
-  </si>
-  <si>
-    <t xml:space="preserve">naaawewe@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">electricaribe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">electricaribe.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">electricidad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aguilera</t>
-  </si>
-  <si>
-    <t xml:space="preserve">costeño</t>
-  </si>
-  <si>
-    <t xml:space="preserve">crcaguilerapo@pornhub.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dfsdfdsf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fvsdfsdfsd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fsdfsdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dsfsdfds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fsdfds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">juanluis@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fgdfgdgdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">club social </t>
-  </si>
-  <si>
-    <t xml:space="preserve">cs.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">porno</t>
-  </si>
-  <si>
-    <t xml:space="preserve">polanco</t>
-  </si>
-  <si>
-    <t xml:space="preserve">crc@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vbgfhfghf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">huawei</t>
-  </si>
-  <si>
-    <t xml:space="preserve">huawei.comm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tecnologia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mike</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sgurt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mark@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fsdfddfsdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">exitooo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">éxito.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eleekk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dsss</t>
-  </si>
-  <si>
-    <t xml:space="preserve">exitooo@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rappi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rappi.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">delivery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mateus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uribe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mateus@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rappi2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mateus2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">correo1@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rappi3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">correo3@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rappi4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gggg@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rappi5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">correo5@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rappi6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">correo6@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rappi7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">correo7@gmail.com</t>
+    <t xml:space="preserve">osomazorca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">osomazorca.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">comidas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oscar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">agudelo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oscar@osomazorca.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toshiba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toshiba.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">computers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mariano</t>
+  </si>
+  <si>
+    <t xml:space="preserve">carreno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mariano@toshiba.com</t>
   </si>
 </sst>
 </file>
@@ -458,7 +326,7 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -518,7 +386,7 @@
         <v>12</v>
       </c>
       <c r="F2" s="4" t="n">
-        <v>4423432</v>
+        <v>3203525634</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>13</v>
@@ -544,7 +412,7 @@
         <v>19</v>
       </c>
       <c r="F3" s="6" t="n">
-        <v>4342343333</v>
+        <v>3112324563</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>20</v>
@@ -570,7 +438,7 @@
         <v>25</v>
       </c>
       <c r="F4" s="6" t="n">
-        <v>5767567</v>
+        <v>3102343267</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>26</v>
@@ -580,291 +448,44 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="7" t="n">
-        <v>43543543</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>33</v>
-      </c>
+      <c r="A5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" s="7" t="n">
-        <v>545345345</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>39</v>
-      </c>
+      <c r="A6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F7" s="7" t="n">
-        <v>53544564</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>46</v>
-      </c>
+      <c r="A7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" s="7" t="n">
-        <v>5454545322</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>14</v>
-      </c>
+      <c r="A8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" s="0" t="n">
-        <v>543545</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="F10" s="0" t="n">
-        <v>543545</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" s="0" t="n">
-        <v>543545</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="F12" s="0" t="n">
-        <v>543545</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="H12" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="F13" s="0" t="n">
-        <v>543545</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="F14" s="0" t="n">
-        <v>543545</v>
-      </c>
-      <c r="G14" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="H14" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="F15" s="0" t="n">
-        <v>543545</v>
-      </c>
-      <c r="G15" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="H15" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1852,20 +1473,9 @@
     <row r="1000" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" display="mauro@gmail.com"/>
-    <hyperlink ref="G3" r:id="rId2" display="naaawewe@gmail.com"/>
-    <hyperlink ref="G4" r:id="rId3" display="crcaguilerapo@pornhub.com"/>
-    <hyperlink ref="G5" r:id="rId4" display="juanluis@gmail.com"/>
-    <hyperlink ref="G6" r:id="rId5" display="crc@gmail.com"/>
-    <hyperlink ref="G7" r:id="rId6" display="mark@gmail.com"/>
-    <hyperlink ref="G8" r:id="rId7" display="exitooo@gmail.com"/>
-    <hyperlink ref="G9" r:id="rId8" display="mateus@gmail.com"/>
-    <hyperlink ref="G10" r:id="rId9" display="correo1@gmail.com"/>
-    <hyperlink ref="G11" r:id="rId10" display="correo3@gmail.com"/>
-    <hyperlink ref="G12" r:id="rId11" display="gggg@gmail.com"/>
-    <hyperlink ref="G13" r:id="rId12" display="correo5@gmail.com"/>
-    <hyperlink ref="G14" r:id="rId13" display="correo6@gmail.com"/>
-    <hyperlink ref="G15" r:id="rId14" display="correo7@gmail.com"/>
+    <hyperlink ref="G2" r:id="rId1" display="mario@puntosamarillo.com"/>
+    <hyperlink ref="G3" r:id="rId2" display="oscar@osomazorca.com"/>
+    <hyperlink ref="G4" r:id="rId3" display="mariano@toshiba.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>

</xml_diff>

<commit_message>
arreglando un error del recolector de errores
</commit_message>
<xml_diff>
--- a/file.xlsx
+++ b/file.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>NOMBRE EMPRESA</t>
   </si>
@@ -69,6 +69,15 @@
   </si>
   <si>
     <t>consultoria</t>
+  </si>
+  <si>
+    <t>PANAMERICANA</t>
+  </si>
+  <si>
+    <t>pananmericana</t>
+  </si>
+  <si>
+    <t>librería</t>
   </si>
 </sst>
 </file>
@@ -510,7 +519,7 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -590,13 +599,22 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="C4" s="6"/>
+      <c r="A4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
+      <c r="H4" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>

</xml_diff>

<commit_message>
agregando integracion con front y upload de excel
</commit_message>
<xml_diff>
--- a/file.xlsx
+++ b/file.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="59">
   <si>
     <t xml:space="preserve">NOMBRE EMPRESA</t>
   </si>
@@ -122,6 +122,81 @@
   </si>
   <si>
     <t xml:space="preserve">GEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">costeños SA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coste.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">comidas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aguilera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">costeñoooo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">agui@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IBM1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibm.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tech</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Martin 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibm2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibm2.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aguilera 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibm3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibm3.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aguilera 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ss@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gays.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">industria porno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">perri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y german</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+327115454</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elespectador@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -396,7 +471,7 @@
   <dimension ref="A1:K1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -548,49 +623,179 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
+      <c r="A5" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>13222</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
+      <c r="A6" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>1500</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
+      <c r="A7" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>13222</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
+      <c r="A8" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>13222</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
+      <c r="A9" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>122324</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1589,6 +1794,11 @@
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" display="aurelio@unillanos.edu.co"/>
     <hyperlink ref="G4" r:id="rId2" display="martin@nestle.com"/>
+    <hyperlink ref="G5" r:id="rId3" display="agui@gmail.com"/>
+    <hyperlink ref="G6" r:id="rId4" display="m@gmail.com"/>
+    <hyperlink ref="G7" r:id="rId5" display="a@gmail.com"/>
+    <hyperlink ref="G8" r:id="rId6" display="ss@gmail.com"/>
+    <hyperlink ref="G9" r:id="rId7" display="elespectador@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>

</xml_diff>

<commit_message>
reparando visualizacion del pais en el nombre del deal
</commit_message>
<xml_diff>
--- a/file.xlsx
+++ b/file.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="238">
   <si>
     <t xml:space="preserve">NOMBRE EMPRESA</t>
   </si>
@@ -204,6 +204,36 @@
     <t xml:space="preserve">clarin3.com</t>
   </si>
   <si>
+    <t xml:space="preserve">Clarin 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">teves4@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Giovanny Universidad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clarin 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">teves5@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clarin 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Giovanny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clarin 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clarin4.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">teves6@gmail.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">CATEGORIA DE INDUSTRIA</t>
   </si>
   <si>
@@ -702,16 +732,10 @@
     <t xml:space="preserve">cycarrenol@unal.edu.co</t>
   </si>
   <si>
-    <t xml:space="preserve">Giovanny</t>
-  </si>
-  <si>
     <t xml:space="preserve">Albarracin</t>
   </si>
   <si>
     <t xml:space="preserve">albarracingiovanny@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Giovanny Universidad</t>
   </si>
   <si>
     <t xml:space="preserve">gfalbarracinr@unal.edu.co</t>
@@ -1003,8 +1027,8 @@
   </sheetPr>
   <dimension ref="A1:M1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L11" activeCellId="0" sqref="L11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1403,40 +1427,172 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="8"/>
-      <c r="K10" s="7"/>
+      <c r="A10" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>3000</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <f aca="false">IFERROR(LOOKUP(K10,Usuarios!D:D,Usuarios!B:B),"")</f>
+        <v>47267351</v>
+      </c>
+      <c r="M10" s="0" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="8"/>
-      <c r="K11" s="7"/>
+      <c r="A11" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>4000</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <f aca="false">IFERROR(LOOKUP(K11,Usuarios!D:D,Usuarios!B:B),"")</f>
+        <v>47267606</v>
+      </c>
+      <c r="M11" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="8"/>
-      <c r="K12" s="7"/>
+      <c r="A12" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>5000</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <f aca="false">IFERROR(LOOKUP(K12,Usuarios!D:D,Usuarios!B:B),"")</f>
+        <v>47256291</v>
+      </c>
+      <c r="M12" s="0" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="8"/>
-      <c r="K13" s="7"/>
+      <c r="A13" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>4000</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <f aca="false">IFERROR(LOOKUP(K13,Usuarios!D:D,Usuarios!B:B),"")</f>
+        <v>47256291</v>
+      </c>
+      <c r="M13" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="8"/>
@@ -2581,6 +2737,10 @@
     <hyperlink ref="H7" r:id="rId6" display="teves@gmail.com"/>
     <hyperlink ref="H8" r:id="rId7" display="teves2@gmail.com"/>
     <hyperlink ref="H9" r:id="rId8" display="teves2@gmail.com"/>
+    <hyperlink ref="H10" r:id="rId9" display="teves4@gmail.com"/>
+    <hyperlink ref="H11" r:id="rId10" display="teves5@gmail.com"/>
+    <hyperlink ref="H12" r:id="rId11" display="teves5@gmail.com"/>
+    <hyperlink ref="H13" r:id="rId12" display="teves6@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>
@@ -2611,22 +2771,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2636,12 +2796,12 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2651,7 +2811,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2661,132 +2821,132 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="11" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="11" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="11" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="11" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="11" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="11" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="11" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="11" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="11" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="11" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="11" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="11" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="11" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="11" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="11" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="11" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="11" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="11" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="11" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="11" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2796,557 +2956,557 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="11" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="11" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="11" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="11" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="11" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="11" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="11" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="11" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="11" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="11" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="11" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="11" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="11" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="11" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="11" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="11" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="11" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="11" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="11" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="11" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="11" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="11" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="11" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="11" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="11" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="11" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="11" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="11" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="11" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="11" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="11" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="11" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="11" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="11" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="11" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="11" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="11" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="11" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="11" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="11" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="11" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="11" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="11" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="11" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="11" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="11" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="11" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="11" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="11" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="11" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="11" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="11" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="11" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="11" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="11" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="11" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="11" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="11" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="11" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="11" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="11" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="11" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="11" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="11" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="11" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="11" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="11" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="11" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="11" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="11" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="11" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="11" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="11" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="11" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="11" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="11" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="11" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="11" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="11" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="11" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="11" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="11" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="11" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="11" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="11" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="11" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="11" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="11" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="11" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="11" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="11" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="11" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="11" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="11" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="11" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="11" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="11" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="11" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="11" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="11" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="11" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="11" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="11" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="11" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="11" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="11" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="11" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="11" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="11" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="11" t="s">
-        <v>201</v>
+        <v>211</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="11" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -3392,46 +3552,46 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3442,10 +3602,10 @@
         <v>47267390</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>1587940872813</v>
@@ -3454,7 +3614,7 @@
         <v>1587940872920</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
       <c r="J2" s="0" t="n">
         <f aca="false">FALSE()</f>
@@ -3479,10 +3639,10 @@
         <v>47267420</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>220</v>
+        <v>230</v>
       </c>
       <c r="G3" s="0" t="n">
         <v>1587941669430</v>
@@ -3491,7 +3651,7 @@
         <v>1587941669952</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
       <c r="J3" s="0" t="n">
         <f aca="false">FALSE()</f>
@@ -3516,16 +3676,16 @@
         <v>47267606</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>22</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>221</v>
+        <v>231</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>222</v>
+        <v>232</v>
       </c>
       <c r="G4" s="0" t="n">
         <v>1587944098433</v>
@@ -3534,7 +3694,7 @@
         <v>1587944098433</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
       <c r="J4" s="0" t="n">
         <f aca="false">FALSE()</f>
@@ -3559,16 +3719,16 @@
         <v>47267522</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>36</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="G5" s="0" t="n">
         <v>1587941937442</v>
@@ -3577,7 +3737,7 @@
         <v>1587941937442</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
       <c r="J5" s="0" t="n">
         <f aca="false">FALSE()</f>
@@ -3602,16 +3762,16 @@
         <v>47256291</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>225</v>
+        <v>65</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>227</v>
+        <v>236</v>
       </c>
       <c r="G6" s="0" t="n">
         <v>1587793278794</v>
@@ -3620,7 +3780,7 @@
         <v>1587793278952</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
       <c r="J6" s="0" t="n">
         <f aca="false">FALSE()</f>
@@ -3645,16 +3805,16 @@
         <v>47267351</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>228</v>
+        <v>61</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
       <c r="G7" s="0" t="n">
         <v>1587940431399</v>
@@ -3663,7 +3823,7 @@
         <v>1587945202983</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
       <c r="J7" s="0" t="n">
         <f aca="false">FALSE()</f>

</xml_diff>

<commit_message>
agregando nota y task al deal
</commit_message>
<xml_diff>
--- a/file.xlsx
+++ b/file.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -10,11 +10,8 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Industrias" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Usuarios" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
-  <definedNames>
-    <definedName function="false" hidden="false" localSheetId="2" name="DatosExternos_1" vbProcedure="false">Usuarios!$A$1:$N$7</definedName>
-  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -25,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="198">
   <si>
     <t xml:space="preserve">NOMBRE EMPRESA</t>
   </si>
@@ -66,195 +63,96 @@
     <t xml:space="preserve">PRODUCTO</t>
   </si>
   <si>
-    <t xml:space="preserve">universidad de los andes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uniandes.edu.co</t>
+    <t xml:space="preserve">NOTA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clarin 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clarin4.com</t>
   </si>
   <si>
     <t xml:space="preserve">E-Learning</t>
   </si>
   <si>
-    <t xml:space="preserve">CO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">camilo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ortiz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+358123456</t>
-  </si>
-  <si>
-    <t xml:space="preserve">camilo@uniandes.edu.co</t>
+    <t xml:space="preserve">Arg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">carlitos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">teves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+5743232323</t>
+  </si>
+  <si>
+    <t xml:space="preserve">teves10@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">appointmentscheduled</t>
   </si>
   <si>
+    <t xml:space="preserve">Giovanny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">una nota</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clarin 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">teves11@gmail.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cristian</t>
   </si>
   <si>
-    <t xml:space="preserve">CG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eltiempo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eltiempo.com</t>
+    <t xml:space="preserve">Clarin 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">teves12@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clarin 13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">teves13@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CATEGORIA DE INDUSTRIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accounting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Airlines/Aviation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alternative Dispute Resolution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alternative Medicine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Animation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apparel &amp; Fashion</t>
   </si>
   <si>
     <t xml:space="preserve">Architecture &amp; Planning</t>
   </si>
   <si>
-    <t xml:space="preserve">pedro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">perez</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+5743232323</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pedro@eltiempo.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">elespectador</t>
-  </si>
-  <si>
-    <t xml:space="preserve">elespectador.com</t>
+    <t xml:space="preserve">Arts and Crafts</t>
   </si>
   <si>
     <t xml:space="preserve">Automotive</t>
   </si>
   <si>
-    <t xml:space="preserve">ESP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cristian Yair</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elespectador 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">elespectador2.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alternative Medicine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pedro2@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Youtube 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">youtube.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">carlos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">osorio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">car@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">clarin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">clarin.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">carlitos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">teves</t>
-  </si>
-  <si>
-    <t xml:space="preserve">teves@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clarin 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">clarin2.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">teves2@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clarin 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">clarin3.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clarin 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">teves4@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Giovanny Universidad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clarin 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">teves5@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clarin 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Giovanny</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clarin 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">clarin4.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">teves6@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CATEGORIA DE INDUSTRIA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accounting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Airlines/Aviation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alternative Dispute Resolution</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Animation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Apparel &amp; Fashion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arts and Crafts</t>
-  </si>
-  <si>
     <t xml:space="preserve">Aviation &amp; Aerospace</t>
   </si>
   <si>
@@ -666,79 +564,58 @@
     <t xml:space="preserve">Writing and Editing</t>
   </si>
   <si>
-    <t xml:space="preserve">Column1.portalId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Column1.ownerId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Column1.type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Column1.firstName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Column1.lastName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Column1.email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Column1.createdAt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Column1.updatedAt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Column1.remoteList</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Column1.hasContactsAccess</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Column1.userIdIncludingInactive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Column1.activeUserId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Column1.isActive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Column1.activeSalesforceId</t>
+    <t xml:space="preserve">portalId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ownerId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">firstName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lastName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">createdAt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">updatedAt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remoteList</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hasContactsAccess</t>
+  </si>
+  <si>
+    <t xml:space="preserve">activeSalesforceId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">activeUserId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isActive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">userIdIncludingInactive</t>
   </si>
   <si>
     <t xml:space="preserve">PERSON</t>
   </si>
   <si>
-    <t xml:space="preserve">crcaguilera@unal.edu.co</t>
+    <t xml:space="preserve">Carreño León</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gaaplex@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">[List]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">albarracingiovanny@hotmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Carreño León</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gaaplex@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Carreño</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cycarrenol@unal.edu.co</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Albarracin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">albarracingiovanny@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gfalbarracinr@unal.edu.co</t>
   </si>
 </sst>
 </file>
@@ -748,7 +625,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -798,6 +675,14 @@
       <b val="true"/>
       <sz val="10"/>
       <color rgb="FF21409A"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF2A6099"/>
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
@@ -867,7 +752,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -896,11 +781,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -908,15 +801,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -983,7 +868,7 @@
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF2A6099"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
@@ -998,44 +883,22 @@
 </styleSheet>
 </file>
 
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="owners_hapikey_22b4e662_5580_4547_bb80_b248d73cd10b" displayName="owners_hapikey_22b4e662_5580_4547_bb80_b248d73cd10b" ref="A1:N7" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:N7"/>
-  <tableColumns count="14">
-    <tableColumn id="1" name="Column1.portalId"/>
-    <tableColumn id="2" name="Column1.ownerId"/>
-    <tableColumn id="3" name="Column1.type"/>
-    <tableColumn id="4" name="Column1.firstName"/>
-    <tableColumn id="5" name="Column1.lastName"/>
-    <tableColumn id="6" name="Column1.email"/>
-    <tableColumn id="7" name="Column1.createdAt"/>
-    <tableColumn id="8" name="Column1.updatedAt"/>
-    <tableColumn id="9" name="Column1.remoteList"/>
-    <tableColumn id="10" name="Column1.hasContactsAccess"/>
-    <tableColumn id="11" name="Column1.userIdIncludingInactive"/>
-    <tableColumn id="12" name="Column1.activeUserId"/>
-    <tableColumn id="13" name="Column1.isActive"/>
-    <tableColumn id="14" name="Column1.activeSalesforceId"/>
-  </tableColumns>
-</table>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M1000"/>
+  <dimension ref="A1:N1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.28"/>
@@ -1045,7 +908,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="18.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="14" style="0" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="15" style="0" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="30" style="0" width="14.43"/>
   </cols>
   <sheetData>
@@ -1089,684 +953,422 @@
       <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="0" t="s">
         <v>15</v>
       </c>
+      <c r="C2" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <f aca="false">L3</f>
+        <v>46846311</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="D3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="E3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="F3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="G3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="0" t="n">
-        <v>500</v>
-      </c>
-      <c r="K2" s="7" t="s">
+      <c r="H3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="0" t="n">
-        <f aca="false">IFERROR(LOOKUP(K2,Usuarios!D:D,Usuarios!B:B),"")</f>
-        <v>47267606</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="J3" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>46846311</v>
+      </c>
+      <c r="M3" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="N3" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="1" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" s="0" t="n">
-        <f aca="false">IFERROR(LOOKUP(K3,Usuarios!D:D,Usuarios!B:B),"")</f>
-        <v>47267606</v>
-      </c>
-      <c r="M3" s="0" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>34</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>29</v>
+        <v>17</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>21</v>
+      <c r="I4" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="J4" s="0" t="n">
-        <v>300</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>36</v>
+        <v>2000</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>28</v>
       </c>
       <c r="L4" s="0" t="n">
-        <f aca="false">IFERROR(LOOKUP(K4,Usuarios!D:D,Usuarios!B:B),"")</f>
-        <v>47267522</v>
+        <v>46846311</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
-        <v>37</v>
+      <c r="A5" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>39</v>
+        <v>15</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="K5" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" s="0" t="n">
-        <v>300</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>36</v>
-      </c>
       <c r="L5" s="0" t="n">
-        <f aca="false">IFERROR(LOOKUP(K5,Usuarios!D:D,Usuarios!B:B),"")</f>
-        <v>47267522</v>
+        <v>46846311</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="J6" s="0" t="n">
-        <v>4444</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="L6" s="0" t="n">
-        <f aca="false">IFERROR(LOOKUP(K6,Usuarios!D:D,Usuarios!B:B),"")</f>
-        <v>47267606</v>
-      </c>
-      <c r="M6" s="0" t="s">
-        <v>31</v>
-      </c>
+      <c r="A6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="6"/>
+      <c r="K6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" s="0" t="n">
-        <v>43434</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="L7" s="0" t="n">
-        <f aca="false">IFERROR(LOOKUP(K7,Usuarios!D:D,Usuarios!B:B),"")</f>
-        <v>47267606</v>
-      </c>
-      <c r="M7" s="0" t="s">
-        <v>23</v>
-      </c>
+      <c r="A7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="6"/>
+      <c r="K7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="J8" s="0" t="n">
-        <v>54656</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="L8" s="0" t="n">
-        <f aca="false">IFERROR(LOOKUP(K8,Usuarios!D:D,Usuarios!B:B),"")</f>
-        <v>47267606</v>
-      </c>
-      <c r="M8" s="0" t="s">
-        <v>31</v>
-      </c>
+      <c r="A8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="6"/>
+      <c r="K8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="J9" s="0" t="n">
-        <v>654654</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="L9" s="0" t="n">
-        <f aca="false">IFERROR(LOOKUP(K9,Usuarios!D:D,Usuarios!B:B),"")</f>
-        <v>47267522</v>
-      </c>
-      <c r="M9" s="0" t="s">
-        <v>23</v>
-      </c>
+      <c r="A9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="6"/>
+      <c r="K9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="J10" s="0" t="n">
-        <v>3000</v>
-      </c>
-      <c r="K10" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="L10" s="0" t="n">
-        <f aca="false">IFERROR(LOOKUP(K10,Usuarios!D:D,Usuarios!B:B),"")</f>
-        <v>47267351</v>
-      </c>
-      <c r="M10" s="0" t="s">
-        <v>31</v>
-      </c>
+      <c r="A10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="6"/>
+      <c r="K10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="J11" s="0" t="n">
-        <v>4000</v>
-      </c>
-      <c r="K11" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="L11" s="0" t="n">
-        <f aca="false">IFERROR(LOOKUP(K11,Usuarios!D:D,Usuarios!B:B),"")</f>
-        <v>47267606</v>
-      </c>
-      <c r="M11" s="0" t="s">
-        <v>23</v>
-      </c>
+      <c r="A11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="6"/>
+      <c r="K11" s="9"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="J12" s="0" t="n">
-        <v>5000</v>
-      </c>
-      <c r="K12" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="L12" s="0" t="n">
-        <f aca="false">IFERROR(LOOKUP(K12,Usuarios!D:D,Usuarios!B:B),"")</f>
-        <v>47256291</v>
-      </c>
-      <c r="M12" s="0" t="s">
-        <v>31</v>
-      </c>
+      <c r="A12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="6"/>
+      <c r="K12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="J13" s="0" t="n">
-        <v>4000</v>
-      </c>
-      <c r="K13" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="L13" s="0" t="n">
-        <f aca="false">IFERROR(LOOKUP(K13,Usuarios!D:D,Usuarios!B:B),"")</f>
-        <v>47256291</v>
-      </c>
-      <c r="M13" s="0" t="s">
-        <v>23</v>
-      </c>
+      <c r="A13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="6"/>
+      <c r="K13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="8"/>
-      <c r="K14" s="7"/>
+      <c r="A14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="8"/>
+      <c r="K14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="8"/>
-      <c r="K15" s="7"/>
+      <c r="A15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="8"/>
+      <c r="K15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="8"/>
-      <c r="K16" s="7"/>
+      <c r="A16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="8"/>
+      <c r="K16" s="9"/>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="8"/>
-      <c r="K17" s="7"/>
+      <c r="A17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="8"/>
+      <c r="K17" s="9"/>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="8"/>
-      <c r="K18" s="7"/>
+      <c r="A18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="8"/>
+      <c r="K18" s="9"/>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="8"/>
-      <c r="K19" s="7"/>
+      <c r="A19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="8"/>
+      <c r="K19" s="9"/>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="8"/>
-      <c r="K20" s="7"/>
+      <c r="A20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="8"/>
+      <c r="K20" s="9"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="8"/>
-      <c r="K21" s="7"/>
+      <c r="A21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="8"/>
+      <c r="K21" s="9"/>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="8"/>
-      <c r="K22" s="7"/>
+      <c r="A22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="8"/>
+      <c r="K22" s="9"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="K23" s="7"/>
+      <c r="A23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="8"/>
+      <c r="K23" s="9"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="K24" s="7"/>
+      <c r="A24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="8"/>
+      <c r="K24" s="9"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="K25" s="7"/>
+      <c r="A25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="8"/>
+      <c r="K25" s="9"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="K26" s="7"/>
+      <c r="K26" s="9"/>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="K27" s="7"/>
+      <c r="K27" s="9"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="K28" s="7"/>
+      <c r="K28" s="9"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="K29" s="7"/>
+      <c r="K29" s="9"/>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="K30" s="7"/>
+      <c r="K30" s="9"/>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="K31" s="7"/>
+      <c r="K31" s="9"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="K32" s="7"/>
+      <c r="K32" s="9"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="K33" s="7"/>
+      <c r="K33" s="9"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="K34" s="7"/>
+      <c r="K34" s="9"/>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="K35" s="7"/>
+      <c r="K35" s="9"/>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="K36" s="7"/>
-    </row>
-    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="K37" s="7"/>
-    </row>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="K38" s="7"/>
-    </row>
-    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="K39" s="7"/>
-    </row>
-    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="K40" s="7"/>
-    </row>
-    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="K41" s="7"/>
-    </row>
-    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="K42" s="7"/>
-    </row>
-    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="K43" s="7"/>
-    </row>
-    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="K44" s="7"/>
-    </row>
-    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="K45" s="7"/>
-    </row>
-    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="K46" s="7"/>
-    </row>
-    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="K47" s="7"/>
-    </row>
-    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="K48" s="7"/>
-    </row>
-    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="K49" s="7"/>
-    </row>
-    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="K50" s="7"/>
-    </row>
+      <c r="K36" s="9"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2703,44 +2305,36 @@
     <row r="984" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="985" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="986" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="987" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="988" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="989" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="990" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="991" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="992" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="993" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="994" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="995" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="996" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="997" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="998" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="999" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1000" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="K2:K50" type="list">
-      <formula1>Usuarios!$D$2:$D$50</formula1>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="K2:K36" type="list">
+      <formula1>#REF!</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C2:C50" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C2:C36" type="list">
       <formula1>Industrias!$A$3:$A$148</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" display="camilo@uniandes.edu.co"/>
-    <hyperlink ref="H3" r:id="rId2" display="pedro@eltiempo.com"/>
-    <hyperlink ref="H4" r:id="rId3" display="pedro@eltiempo.com"/>
-    <hyperlink ref="H5" r:id="rId4" display="pedro2@gmail.com"/>
-    <hyperlink ref="H6" r:id="rId5" display="car@gmail.com"/>
-    <hyperlink ref="H7" r:id="rId6" display="teves@gmail.com"/>
-    <hyperlink ref="H8" r:id="rId7" display="teves2@gmail.com"/>
-    <hyperlink ref="H9" r:id="rId8" display="teves2@gmail.com"/>
-    <hyperlink ref="H10" r:id="rId9" display="teves4@gmail.com"/>
-    <hyperlink ref="H11" r:id="rId10" display="teves5@gmail.com"/>
-    <hyperlink ref="H12" r:id="rId11" display="teves5@gmail.com"/>
-    <hyperlink ref="H13" r:id="rId12" display="teves6@gmail.com"/>
+    <hyperlink ref="H2" r:id="rId1" display="teves10@gmail.com"/>
+    <hyperlink ref="H3" r:id="rId2" display="teves11@gmail.com"/>
+    <hyperlink ref="H4" r:id="rId3" display="teves12@gmail.com"/>
+    <hyperlink ref="H5" r:id="rId4" display="teves13@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>
@@ -2759,8 +2353,8 @@
   </sheetPr>
   <dimension ref="A1:A148"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A100" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2771,742 +2365,742 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>69</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
-        <v>70</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
-        <v>72</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="s">
-        <v>74</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="s">
-        <v>76</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>77</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>78</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>79</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>80</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="11" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11" t="s">
-        <v>82</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="11" t="s">
-        <v>83</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="11" t="s">
-        <v>84</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="11" t="s">
-        <v>85</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="11" t="s">
-        <v>86</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="11" t="s">
-        <v>87</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="11" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="11" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="11" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="11" t="s">
-        <v>91</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="11" t="s">
-        <v>92</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="11" t="s">
-        <v>93</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="11" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="11" t="s">
-        <v>95</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="11" t="s">
-        <v>96</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="11" t="s">
-        <v>97</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="11" t="s">
-        <v>98</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="11" t="s">
-        <v>99</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="11" t="s">
-        <v>100</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="11" t="s">
-        <v>101</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="11" t="s">
-        <v>102</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="11" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="11" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="11" t="s">
-        <v>105</v>
+        <v>72</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="11" t="s">
-        <v>106</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="11" t="s">
-        <v>107</v>
+        <v>74</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="11" t="s">
-        <v>108</v>
+        <v>75</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="11" t="s">
-        <v>109</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="11" t="s">
-        <v>110</v>
+        <v>77</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="11" t="s">
-        <v>111</v>
+        <v>78</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="11" t="s">
-        <v>112</v>
+        <v>79</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="11" t="s">
-        <v>113</v>
+        <v>80</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="11" t="s">
-        <v>114</v>
+        <v>81</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="11" t="s">
-        <v>115</v>
+        <v>82</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="11" t="s">
-        <v>116</v>
+        <v>83</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="11" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="11" t="s">
-        <v>118</v>
+        <v>85</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="11" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="11" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="11" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="11" t="s">
-        <v>122</v>
+        <v>89</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="11" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="11" t="s">
-        <v>124</v>
+        <v>91</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="11" t="s">
-        <v>125</v>
+        <v>92</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="11" t="s">
-        <v>126</v>
+        <v>93</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="11" t="s">
-        <v>127</v>
+        <v>94</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="11" t="s">
-        <v>128</v>
+        <v>95</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="11" t="s">
-        <v>129</v>
+        <v>96</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="11" t="s">
-        <v>130</v>
+        <v>97</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="11" t="s">
-        <v>131</v>
+        <v>98</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="11" t="s">
-        <v>132</v>
+        <v>99</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="11" t="s">
-        <v>133</v>
+        <v>100</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="11" t="s">
-        <v>134</v>
+        <v>101</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="11" t="s">
-        <v>135</v>
+        <v>102</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="11" t="s">
-        <v>136</v>
+        <v>103</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="11" t="s">
-        <v>137</v>
+        <v>104</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="11" t="s">
-        <v>138</v>
+        <v>105</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="11" t="s">
-        <v>139</v>
+        <v>106</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="11" t="s">
-        <v>140</v>
+        <v>107</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="11" t="s">
-        <v>141</v>
+        <v>108</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="11" t="s">
-        <v>142</v>
+        <v>109</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="11" t="s">
-        <v>143</v>
+        <v>110</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="11" t="s">
-        <v>144</v>
+        <v>111</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="11" t="s">
-        <v>145</v>
+        <v>112</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="11" t="s">
-        <v>146</v>
+        <v>113</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="11" t="s">
-        <v>147</v>
+        <v>114</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="11" t="s">
-        <v>148</v>
+        <v>115</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="11" t="s">
-        <v>149</v>
+        <v>116</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="11" t="s">
-        <v>150</v>
+        <v>117</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="11" t="s">
-        <v>151</v>
+        <v>118</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="11" t="s">
-        <v>152</v>
+        <v>119</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="11" t="s">
-        <v>153</v>
+        <v>120</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="11" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="11" t="s">
-        <v>155</v>
+        <v>122</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="11" t="s">
-        <v>156</v>
+        <v>123</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="11" t="s">
-        <v>157</v>
+        <v>124</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="11" t="s">
-        <v>158</v>
+        <v>125</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="11" t="s">
-        <v>159</v>
+        <v>126</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="11" t="s">
-        <v>160</v>
+        <v>127</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="11" t="s">
-        <v>161</v>
+        <v>128</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="11" t="s">
-        <v>162</v>
+        <v>129</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="11" t="s">
-        <v>163</v>
+        <v>130</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="11" t="s">
-        <v>164</v>
+        <v>131</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="11" t="s">
-        <v>165</v>
+        <v>132</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="11" t="s">
-        <v>166</v>
+        <v>133</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="11" t="s">
-        <v>167</v>
+        <v>134</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="11" t="s">
-        <v>168</v>
+        <v>135</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="11" t="s">
-        <v>169</v>
+        <v>136</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="11" t="s">
-        <v>170</v>
+        <v>137</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="11" t="s">
-        <v>171</v>
+        <v>138</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="11" t="s">
-        <v>172</v>
+        <v>139</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="11" t="s">
-        <v>173</v>
+        <v>140</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="11" t="s">
-        <v>174</v>
+        <v>141</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="11" t="s">
-        <v>175</v>
+        <v>142</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="11" t="s">
-        <v>176</v>
+        <v>143</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="11" t="s">
-        <v>177</v>
+        <v>144</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="11" t="s">
-        <v>178</v>
+        <v>145</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="11" t="s">
-        <v>179</v>
+        <v>146</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="11" t="s">
-        <v>180</v>
+        <v>147</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="11" t="s">
-        <v>181</v>
+        <v>148</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="11" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="11" t="s">
-        <v>183</v>
+        <v>150</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="11" t="s">
-        <v>184</v>
+        <v>151</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="11" t="s">
-        <v>185</v>
+        <v>152</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="11" t="s">
-        <v>186</v>
+        <v>153</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="11" t="s">
-        <v>187</v>
+        <v>154</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="11" t="s">
-        <v>188</v>
+        <v>155</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="11" t="s">
-        <v>189</v>
+        <v>156</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="11" t="s">
-        <v>190</v>
+        <v>157</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="11" t="s">
-        <v>191</v>
+        <v>158</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="11" t="s">
-        <v>192</v>
+        <v>159</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="11" t="s">
-        <v>193</v>
+        <v>160</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="11" t="s">
-        <v>194</v>
+        <v>161</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="11" t="s">
-        <v>195</v>
+        <v>162</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="11" t="s">
-        <v>196</v>
+        <v>163</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="11" t="s">
-        <v>197</v>
+        <v>164</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="11" t="s">
-        <v>198</v>
+        <v>165</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="11" t="s">
-        <v>199</v>
+        <v>166</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="11" t="s">
-        <v>200</v>
+        <v>167</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="11" t="s">
-        <v>201</v>
+        <v>168</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="11" t="s">
-        <v>202</v>
+        <v>169</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="11" t="s">
-        <v>203</v>
+        <v>170</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="11" t="s">
-        <v>204</v>
+        <v>171</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="11" t="s">
-        <v>205</v>
+        <v>172</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="11" t="s">
-        <v>206</v>
+        <v>173</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="11" t="s">
-        <v>207</v>
+        <v>174</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="11" t="s">
-        <v>208</v>
+        <v>175</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="11" t="s">
-        <v>209</v>
+        <v>176</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="11" t="s">
-        <v>210</v>
+        <v>177</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="11" t="s">
-        <v>211</v>
+        <v>178</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="11" t="s">
-        <v>212</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -3525,332 +3119,112 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="28.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="21.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="29.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="33.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="23.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="28.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="10.65"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>7579777</v>
+        <v>7524382</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>47267390</v>
+        <v>46846311</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>227</v>
+        <v>194</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>195</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>228</v>
+        <v>196</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>1587940872813</v>
+        <v>1587093015986</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>1587940872920</v>
+        <v>1587093015986</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>229</v>
+        <v>197</v>
       </c>
       <c r="J2" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="K2" s="0" t="n">
-        <v>10621710</v>
-      </c>
       <c r="L2" s="0" t="n">
-        <v>10621710</v>
+        <v>10532486</v>
       </c>
       <c r="M2" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>7579777</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>47267420</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>227</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>230</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>1587941669430</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>1587941669952</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K3" s="0" t="n">
-        <v>10621763</v>
-      </c>
-      <c r="L3" s="0" t="n">
-        <v>10621763</v>
-      </c>
-      <c r="M3" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>7579777</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>47267606</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>227</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>231</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>232</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>1587944098433</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>1587944098433</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K4" s="0" t="n">
+      <c r="N2" s="0" t="n">
         <v>10532486</v>
-      </c>
-      <c r="L4" s="0" t="n">
-        <v>10532486</v>
-      </c>
-      <c r="M4" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>7579777</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>47267522</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>227</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>233</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>234</v>
-      </c>
-      <c r="G5" s="0" t="n">
-        <v>1587941937442</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <v>1587941937442</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="J5" s="0" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K5" s="0" t="n">
-        <v>10556931</v>
-      </c>
-      <c r="L5" s="0" t="n">
-        <v>10556931</v>
-      </c>
-      <c r="M5" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>7579777</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>47256291</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>227</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>235</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>236</v>
-      </c>
-      <c r="G6" s="0" t="n">
-        <v>1587793278794</v>
-      </c>
-      <c r="H6" s="0" t="n">
-        <v>1587793278952</v>
-      </c>
-      <c r="I6" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="J6" s="0" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K6" s="0" t="n">
-        <v>10612193</v>
-      </c>
-      <c r="L6" s="0" t="n">
-        <v>10612193</v>
-      </c>
-      <c r="M6" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>7579777</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>47267351</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>227</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>235</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>237</v>
-      </c>
-      <c r="G7" s="0" t="n">
-        <v>1587940431399</v>
-      </c>
-      <c r="H7" s="0" t="n">
-        <v>1587945202983</v>
-      </c>
-      <c r="I7" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="J7" s="0" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K7" s="0" t="n">
-        <v>10621689</v>
-      </c>
-      <c r="L7" s="0" t="n">
-        <v>10621689</v>
-      </c>
-      <c r="M7" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <tableParts>
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>